<commit_message>
UART and PWM working
</commit_message>
<xml_diff>
--- a/DOC/DMX_CTRL.xlsx
+++ b/DOC/DMX_CTRL.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20295" windowHeight="12255" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20295" windowHeight="12255" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
     <sheet name="Commands" sheetId="2" r:id="rId2"/>
-    <sheet name="Links" sheetId="3" r:id="rId3"/>
+    <sheet name="Control Methods" sheetId="5" r:id="rId3"/>
+    <sheet name="FX List" sheetId="4" r:id="rId4"/>
+    <sheet name="Links" sheetId="3" r:id="rId5"/>
+    <sheet name="Ressource Allocation" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -20,8 +23,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Windows User</author>
+  </authors>
+  <commentList>
+    <comment ref="C52" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Wy 183… Because we don't want to use a code with a high frequency (0,255,128,63…) as each substitution creates overhead….
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="225">
   <si>
     <t>Pin</t>
   </si>
@@ -275,15 +313,6 @@
     <t>STRIP1_COMPLEXITY</t>
   </si>
   <si>
-    <t>STRIP1_R</t>
-  </si>
-  <si>
-    <t>STRIP1_G</t>
-  </si>
-  <si>
-    <t>STRIP1_B</t>
-  </si>
-  <si>
     <t>STRIP2_PATTERN</t>
   </si>
   <si>
@@ -296,15 +325,6 @@
     <t>STRIP2_COMPLEXITY</t>
   </si>
   <si>
-    <t>STRIP2_R</t>
-  </si>
-  <si>
-    <t>STRIP2_G</t>
-  </si>
-  <si>
-    <t>STRIP2_B</t>
-  </si>
-  <si>
     <t>Bitfield for options</t>
   </si>
   <si>
@@ -420,13 +440,307 @@
   </si>
   <si>
     <t>Master/Slave</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Solid Color (Or Off)</t>
+  </si>
+  <si>
+    <t>Hue</t>
+  </si>
+  <si>
+    <t>Brightness</t>
+  </si>
+  <si>
+    <t>Saturation</t>
+  </si>
+  <si>
+    <t>Solid Color</t>
+  </si>
+  <si>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>STRIP1_V1</t>
+  </si>
+  <si>
+    <t>STRIP1_V2</t>
+  </si>
+  <si>
+    <t>STRIP1_V3</t>
+  </si>
+  <si>
+    <t>STRIP2_V1</t>
+  </si>
+  <si>
+    <t>STRIP2_V2</t>
+  </si>
+  <si>
+    <t>STRIP2_V3</t>
+  </si>
+  <si>
+    <t>Scrollspeed</t>
+  </si>
+  <si>
+    <t>Stepsize</t>
+  </si>
+  <si>
+    <t>Rainbow</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>Cylon Eye Red Dot Ping Pong</t>
+  </si>
+  <si>
+    <t>Cylon Eye Red Dot Wrap-Around</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>https://github.com/rogerclarkmelbourne/Arduino_STM32/tree/master/STM32F1/libraries/WS2812B</t>
+  </si>
+  <si>
+    <t>1) DMX512</t>
+  </si>
+  <si>
+    <t>3) USB Virtual Serial Port</t>
+  </si>
+  <si>
+    <t>Pro</t>
+  </si>
+  <si>
+    <t>Multiple devices in Parallel on same Link</t>
+  </si>
+  <si>
+    <t>Combine Data + Power in 4-Pin Cable</t>
+  </si>
+  <si>
+    <t>Con</t>
+  </si>
+  <si>
+    <t>Protocol Hard to implement on PC</t>
+  </si>
+  <si>
+    <t>Overkill for Individual Devices</t>
+  </si>
+  <si>
+    <t>Easy to connect to PC</t>
+  </si>
+  <si>
+    <t>Harder to control via PC, needs specialized HW and software</t>
+  </si>
+  <si>
+    <t>Easy to Control</t>
+  </si>
+  <si>
+    <t>Timing is kind of tricky to get right</t>
+  </si>
+  <si>
+    <t>Industry-Standard</t>
+  </si>
+  <si>
+    <t>Devices can be chained up</t>
+  </si>
+  <si>
+    <t>RS485 allows for long cables</t>
+  </si>
+  <si>
+    <t>Limited cable range on RS232</t>
+  </si>
+  <si>
+    <t>Lower Data rate</t>
+  </si>
+  <si>
+    <t>Datarate limits registers to 512, refresh rate to 44FPS</t>
+  </si>
+  <si>
+    <t>2) UART (155200 Baud, 8N1)</t>
+  </si>
+  <si>
+    <t>High Data Rate</t>
+  </si>
+  <si>
+    <t>Only one device per USB port (But can use Hubs)</t>
+  </si>
+  <si>
+    <t>Compatible with UART implementation</t>
+  </si>
+  <si>
+    <t>4) Wifi via ESP8266 (ESP-01 Module)</t>
+  </si>
+  <si>
+    <t>Wireless</t>
+  </si>
+  <si>
+    <t>Allows for Webserver Implementation</t>
+  </si>
+  <si>
+    <t>Hard to syncronize Timing</t>
+  </si>
+  <si>
+    <t>Hard to implement</t>
+  </si>
+  <si>
+    <t>Protocol Details</t>
+  </si>
+  <si>
+    <t>DMX512</t>
+  </si>
+  <si>
+    <t>DMX512 Compliant Protocol Parsing</t>
+  </si>
+  <si>
+    <t>UART</t>
+  </si>
+  <si>
+    <t>Hard to signal start of packet</t>
+  </si>
+  <si>
+    <t>Option 1) Challenge/Response. Slave sends character whenever it is ready to receive another 512 Byte packet.</t>
+  </si>
+  <si>
+    <t>Same Protocol as UART</t>
+  </si>
+  <si>
+    <t>Wifi</t>
+  </si>
+  <si>
+    <t>Oprion 3) Timing based. Leave a gap in transmission at the start of new packet as DMX512 does. Hard to do for example for USB and Wifi</t>
+  </si>
+  <si>
+    <t>Interface Options</t>
+  </si>
+  <si>
+    <t>At 115200 Baud we are limited in refresh rate to a maximum of 28 FPS. (Can theoretically go to higher baud rates)</t>
+  </si>
+  <si>
+    <t>Escape Code Sequence</t>
+  </si>
+  <si>
+    <t>Start Code</t>
+  </si>
+  <si>
+    <t>Start of packet</t>
+  </si>
+  <si>
+    <t>0x5C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Option 2) Escaped code sequence. Creates data overhead. On specific code (0x5C '\') the next character is interpreted as type (start of packet, config command, normal char 0X01..) </t>
+  </si>
+  <si>
+    <t>0x6D</t>
+  </si>
+  <si>
+    <t>Enter config mode (So manually typing '\m' gets one into menu/debug mode</t>
+  </si>
+  <si>
+    <t>Substitute with 0x5C (The escape character)</t>
+  </si>
+  <si>
+    <t>Can potentially directly implement ArtNET</t>
+  </si>
+  <si>
+    <t>Potential for direct ArtNET communication</t>
+  </si>
+  <si>
+    <t>Hardware Modules</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>UART 1</t>
+  </si>
+  <si>
+    <t>UART 3</t>
+  </si>
+  <si>
+    <t>TIM1</t>
+  </si>
+  <si>
+    <t>IWDT</t>
+  </si>
+  <si>
+    <t>Watch Dog Timer</t>
+  </si>
+  <si>
+    <t>DMA</t>
+  </si>
+  <si>
+    <t>Drive SPI/WS2812B Output</t>
+  </si>
+  <si>
+    <t>SPI1</t>
+  </si>
+  <si>
+    <t>WS2812B Ch1</t>
+  </si>
+  <si>
+    <t>SPI2</t>
+  </si>
+  <si>
+    <t>WS2812B Ch2</t>
+  </si>
+  <si>
+    <t>CH3 PWM</t>
+  </si>
+  <si>
+    <t>TIM2</t>
+  </si>
+  <si>
+    <t>TIM3</t>
+  </si>
+  <si>
+    <t>CH2 PWM</t>
+  </si>
+  <si>
+    <t>CH1 PWM</t>
+  </si>
+  <si>
+    <t>TIM4</t>
+  </si>
+  <si>
+    <t>Reserved fro DMX512 Timing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -467,6 +781,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -520,7 +847,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -533,6 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1044,8 +1372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A14:A17"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1104,7 +1432,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
@@ -1115,7 +1443,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
@@ -1126,7 +1454,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
@@ -1137,7 +1465,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
@@ -1148,7 +1476,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
@@ -1167,7 +1495,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
         <v>47</v>
@@ -1178,7 +1506,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
         <v>47</v>
@@ -1189,7 +1517,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
@@ -1200,7 +1528,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
@@ -1233,7 +1561,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
@@ -1255,7 +1583,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
         <v>50</v>
@@ -1277,7 +1605,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
         <v>48</v>
@@ -1288,7 +1616,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
         <v>48</v>
@@ -1299,7 +1627,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
         <v>48</v>
@@ -1326,7 +1654,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
@@ -1337,7 +1665,7 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
         <v>50</v>
@@ -1370,10 +1698,10 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1381,7 +1709,7 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1389,7 +1717,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C35" t="s">
         <v>50</v>
@@ -1397,10 +1725,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C36" t="s">
         <v>50</v>
@@ -1415,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1426,15 +1754,15 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
-        <v>95</v>
+      <c r="B3" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1533,10 +1861,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1576,7 +1904,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>84</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1584,7 +1912,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1592,7 +1920,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1600,7 +1928,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1608,7 +1936,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1616,7 +1944,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1624,7 +1952,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1632,7 +1960,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>91</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1640,7 +1968,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>92</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1648,55 +1976,55 @@
         <v>25</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>93</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="4" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="2:5">
@@ -1704,7 +2032,7 @@
         <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="2:5">
@@ -1717,7 +2045,7 @@
         <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="2:2">
@@ -1728,17 +2056,474 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:A20"/>
+  <dimension ref="A1:C67"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="3" max="3" width="75.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="C10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="C13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="C18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="C19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="C20" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="C22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="C23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="C27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="C28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="C29" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="C31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="B34" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="C35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="C36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="C37" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="C39" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="C40" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="B49" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="B50" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="C51" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="C52" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="C53" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="B59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>198</v>
+      </c>
+      <c r="B63" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>131</v>
+      </c>
+      <c r="B65" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>198</v>
+      </c>
+      <c r="B66" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>200</v>
+      </c>
+      <c r="B67" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="8" max="8" width="50.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>155</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="H7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A5:A21"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1783,30 +2568,144 @@
         <v>62</v>
       </c>
     </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>63</v>
-      </c>
+      <c r="A17" s="3"/>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" s="3" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A20" r:id="rId1"/>
+    <hyperlink ref="A21" r:id="rId1"/>
+    <hyperlink ref="A16" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:B17"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FX Mananger Framework added
</commit_message>
<xml_diff>
--- a/DOC/DMX_CTRL.xlsx
+++ b/DOC/DMX_CTRL.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="20295" windowHeight="12255" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20295" windowHeight="12255" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,9 @@
     <sheet name="Links" sheetId="3" r:id="rId5"/>
     <sheet name="Ressource Allocation" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="145621"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="237">
   <si>
     <t>Pin</t>
   </si>
@@ -325,9 +325,6 @@
     <t>STRIP2_COMPLEXITY</t>
   </si>
   <si>
-    <t>Bitfield for options</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -346,9 +343,6 @@
     <t>Option 4</t>
   </si>
   <si>
-    <t>STRIP_BITS</t>
-  </si>
-  <si>
     <t>Minimum 4 Bytes, Max 26 Bytes Address Space</t>
   </si>
   <si>
@@ -734,13 +728,55 @@
   </si>
   <si>
     <t>Reserved fro DMX512 Timing</t>
+  </si>
+  <si>
+    <t>FX_SELECT</t>
+  </si>
+  <si>
+    <t>Effect Selection</t>
+  </si>
+  <si>
+    <t>Variables for Strip 1</t>
+  </si>
+  <si>
+    <t>Variables for Strip 2</t>
+  </si>
+  <si>
+    <t>Effects are selected via the FX_SELECT Register</t>
+  </si>
+  <si>
+    <t>Effects can control PWM Lights or Strips or both</t>
+  </si>
+  <si>
+    <t>Effects are only available with extended register space</t>
+  </si>
+  <si>
+    <t>PWM Lights shall be controlled by modifying registers from the Effect</t>
+  </si>
+  <si>
+    <t>Only one effect can be running at any time</t>
+  </si>
+  <si>
+    <t>Two Sets of Variables are provided so Pattern and other parameter can vary between the two strips</t>
+  </si>
+  <si>
+    <t>Effects can run continuous until another effect is selected</t>
+  </si>
+  <si>
+    <t>Effect can run in different modes</t>
+  </si>
+  <si>
+    <t>Effects can run Once and then the system falls back to the last effect (Single Shot)</t>
+  </si>
+  <si>
+    <t>Effects can run in Loop mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -904,7 +940,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{03A9691C-02CA-4C40-9132-87F05A099AD9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03A9691C-02CA-4C40-9132-87F05A099AD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1362,31 +1398,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C36"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="18.75">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1394,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1405,7 +1441,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -1416,7 +1452,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1427,62 +1463,62 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1490,51 +1526,51 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
@@ -1545,7 +1581,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
@@ -1556,18 +1592,18 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -1578,18 +1614,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
@@ -1600,40 +1636,40 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -1641,7 +1677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
@@ -1649,29 +1685,29 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>28</v>
       </c>
@@ -1682,7 +1718,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>29</v>
       </c>
@@ -1693,42 +1729,42 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
         <v>50</v>
@@ -1740,32 +1776,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1776,7 +1812,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1784,7 +1820,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1792,7 +1828,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1800,7 +1836,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1808,7 +1844,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1816,7 +1852,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1824,7 +1860,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1832,7 +1868,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1840,7 +1876,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1848,7 +1884,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1856,26 +1892,29 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>95</v>
+        <v>223</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1883,7 +1922,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1891,7 +1930,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1899,39 +1938,42 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1939,7 +1981,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1947,7 +1989,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1955,103 +1997,103 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="s">
         <v>96</v>
       </c>
-      <c r="E33" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" t="s">
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" t="s">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="C40" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="10"/>
     </row>
-    <row r="51" spans="2:2">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="11"/>
     </row>
   </sheetData>
@@ -2062,303 +2104,303 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="75.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="C5" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="C6" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="C7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="C8" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="C10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="C11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="C12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="C13" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="C14" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="B17" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="C18" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="C19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="C20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="B21" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="C22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="C23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="B26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="C27" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="C28" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="C29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="B30" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="C31" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="B34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="C35" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="C36" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
-      <c r="C37" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="B38" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="C39" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="C40" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="B46" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="B49" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="B50" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="C51" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>196</v>
+      </c>
+      <c r="B63" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>196</v>
+      </c>
+      <c r="B66" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>198</v>
       </c>
-      <c r="B63" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
-        <v>131</v>
-      </c>
-      <c r="B65" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
-        <v>198</v>
-      </c>
-      <c r="B66" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
-        <v>200</v>
-      </c>
       <c r="B67" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2368,148 +2410,198 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="50.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
         <v>127</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>128</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>129</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B3" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C3" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H3" t="s">
         <v>135</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="F4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="H5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="F6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" t="s">
         <v>134</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" t="s">
-        <v>139</v>
-      </c>
-      <c r="H4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" t="s">
-        <v>139</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" t="s">
-        <v>136</v>
-      </c>
-      <c r="H6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="H7" t="s">
-        <v>153</v>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2519,79 +2611,79 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:A21"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>66</v>
       </c>
@@ -2606,103 +2698,103 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>207</v>
-      </c>
       <c r="B3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" t="s">
         <v>209</v>
       </c>
-      <c r="B6" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>219</v>
-      </c>
-      <c r="B7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>220</v>
-      </c>
-      <c r="B8" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>223</v>
-      </c>
-      <c r="B9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>214</v>
-      </c>
-      <c r="B11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>210</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Serial DMX Protocol
All WIP...
</commit_message>
<xml_diff>
--- a/DOC/DMX_CTRL.xlsx
+++ b/DOC/DMX_CTRL.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael.Hartmann\Documents\GitHub\DMX_CTRL\DOC\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="20295" windowHeight="12255" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20295" windowHeight="12255" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="C52" authorId="0">
+    <comment ref="C53" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="238">
   <si>
     <t>Pin</t>
   </si>
@@ -637,9 +642,6 @@
     <t>Interface Options</t>
   </si>
   <si>
-    <t>At 115200 Baud we are limited in refresh rate to a maximum of 28 FPS. (Can theoretically go to higher baud rates)</t>
-  </si>
-  <si>
     <t>Escape Code Sequence</t>
   </si>
   <si>
@@ -770,12 +772,18 @@
   </si>
   <si>
     <t>Effects can run in Loop mode</t>
+  </si>
+  <si>
+    <t>At 115200 Baud we are limited in refresh rate to a maximum of 28 FPS if we send the full 512 registers. (Can theoretically go to higher baud rates)</t>
+  </si>
+  <si>
+    <t>Or we only send the registers nessassary as UART will be a point-to-point connection….</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -940,7 +948,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03A9691C-02CA-4C40-9132-87F05A099AD9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03A9691C-02CA-4C40-9132-87F05A099AD9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1398,7 +1406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1897,10 +1905,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" t="s">
         <v>223</v>
-      </c>
-      <c r="C15" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1911,7 +1919,7 @@
         <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1970,7 +1978,7 @@
         <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2105,10 +2113,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2278,7 +2286,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2318,89 +2326,94 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>192</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>193</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>196</v>
-      </c>
-      <c r="B63" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>129</v>
-      </c>
-      <c r="B65" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>195</v>
+      </c>
+      <c r="B64" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B67" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>197</v>
+      </c>
+      <c r="B68" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2413,7 +2426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2556,52 +2569,52 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2709,12 +2722,12 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s">
         <v>183</v>
@@ -2722,7 +2735,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -2730,71 +2743,71 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" t="s">
         <v>218</v>
-      </c>
-      <c r="B8" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" t="s">
         <v>221</v>
-      </c>
-      <c r="B9" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" t="s">
         <v>212</v>
-      </c>
-      <c r="B11" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>213</v>
+      </c>
+      <c r="B12" t="s">
         <v>214</v>
-      </c>
-      <c r="B12" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" t="s">
         <v>208</v>
-      </c>
-      <c r="B14" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" t="s">
         <v>210</v>
-      </c>
-      <c r="B15" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cylon example , update docu
</commit_message>
<xml_diff>
--- a/DOC/DMX_CTRL.xlsx
+++ b/DOC/DMX_CTRL.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="20295" windowHeight="12255" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20295" windowHeight="12255"/>
   </bookViews>
   <sheets>
-    <sheet name="Pinout" sheetId="1" r:id="rId1"/>
-    <sheet name="Commands" sheetId="2" r:id="rId2"/>
-    <sheet name="Control Methods" sheetId="5" r:id="rId3"/>
-    <sheet name="FX List" sheetId="4" r:id="rId4"/>
-    <sheet name="Links" sheetId="3" r:id="rId5"/>
-    <sheet name="Ressource Allocation" sheetId="6" r:id="rId6"/>
+    <sheet name="Intro" sheetId="7" r:id="rId1"/>
+    <sheet name="Pinout" sheetId="1" r:id="rId2"/>
+    <sheet name="Commands" sheetId="2" r:id="rId3"/>
+    <sheet name="Control Methods" sheetId="5" r:id="rId4"/>
+    <sheet name="FX List" sheetId="4" r:id="rId5"/>
+    <sheet name="Links" sheetId="3" r:id="rId6"/>
+    <sheet name="Ressource Allocation" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="228">
   <si>
     <t>Pin</t>
   </si>
@@ -336,42 +337,6 @@
     <t>DMX Command Bytes</t>
   </si>
   <si>
-    <t>Option 1</t>
-  </si>
-  <si>
-    <t>Option 2</t>
-  </si>
-  <si>
-    <t>Option 3</t>
-  </si>
-  <si>
-    <t>Option 4</t>
-  </si>
-  <si>
-    <t>Minimum 4 Bytes, Max 26 Bytes Address Space</t>
-  </si>
-  <si>
-    <t>(Max 128 min 20 Devices/Universe…)</t>
-  </si>
-  <si>
-    <t>RGBW LED/Strip (Or Simple RGB…)</t>
-  </si>
-  <si>
-    <t>RGB LED/Strip or YPR Motor Control</t>
-  </si>
-  <si>
-    <t>RGB LED/Strip With Maximum Scaled Brightness</t>
-  </si>
-  <si>
-    <t>Option 5</t>
-  </si>
-  <si>
-    <t>WS8212 Strip</t>
-  </si>
-  <si>
-    <t>When pressed while connecting to USB goes into serial port confirugration mode to set options. When Pressed during operation goes into test mode</t>
-  </si>
-  <si>
     <t>I2C1_SCL / ADDR 3</t>
   </si>
   <si>
@@ -438,9 +403,6 @@
     <t>PWM CH2 B (PWM1/3)</t>
   </si>
   <si>
-    <t>Master/Slave</t>
-  </si>
-  <si>
     <t>Pattern</t>
   </si>
   <si>
@@ -778,13 +740,22 @@
   </si>
   <si>
     <t>Or we only send the registers nessassary as UART will be a point-to-point connection….</t>
+  </si>
+  <si>
+    <t>Control Button</t>
+  </si>
+  <si>
+    <t>RS485 Direction Selection (In/Out)</t>
+  </si>
+  <si>
+    <t>This is just a collection of initial thoughts/ideas and probably outdated by now !!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -839,25 +810,27 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -867,14 +840,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB8B3FF"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -887,26 +858,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -932,16 +905,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -956,8 +929,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="850900" y="9423400"/>
-          <a:ext cx="9296400" cy="5613400"/>
+          <a:off x="349250" y="6057900"/>
+          <a:ext cx="9410700" cy="4676775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1056,7 +1029,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-	2 Mode Jumpers to hard-select options (Master/Slave and WS8212 Support on/off ?)</a:t>
+            <a:t>-	2 Mode Jumpers to hard-select options </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1414,10 +1387,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1432,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -1450,7 +1443,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -1461,7 +1454,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -1472,114 +1465,117 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>41</v>
       </c>
+      <c r="C13" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C16" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -1590,7 +1586,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -1601,18 +1597,18 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -1623,18 +1619,18 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -1645,40 +1641,40 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -1686,7 +1682,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -1694,29 +1690,29 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B31" t="s">
@@ -1727,7 +1723,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B32" t="s">
@@ -1738,41 +1734,44 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C35" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>113</v>
+      <c r="A36" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
         <v>50</v>
@@ -1783,12 +1782,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1813,7 +1812,7 @@
       <c r="A4">
         <v>0</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="s">
@@ -1824,7 +1823,7 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="9" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1832,7 +1831,7 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="9" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1840,7 +1839,7 @@
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="9" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1848,7 +1847,7 @@
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1856,7 +1855,7 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1864,7 +1863,7 @@
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="9" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1872,7 +1871,7 @@
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="9" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1880,7 +1879,7 @@
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="9" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1888,7 +1887,7 @@
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="9" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1896,7 +1895,7 @@
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="9" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1904,29 +1903,29 @@
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>222</v>
+      <c r="B15" s="10" t="s">
+        <v>209</v>
       </c>
       <c r="C15" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="10" t="s">
         <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="10" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1934,7 +1933,7 @@
       <c r="A18">
         <v>14</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="10" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1942,7 +1941,7 @@
       <c r="A19">
         <v>15</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="10" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1950,42 +1949,42 @@
       <c r="A20">
         <v>16</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>141</v>
+      <c r="B20" s="10" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>142</v>
+      <c r="B21" s="10" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>143</v>
+      <c r="B22" s="10" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="10" t="s">
         <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="10" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1993,7 +1992,7 @@
       <c r="A25">
         <v>21</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="10" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2001,7 +2000,7 @@
       <c r="A26">
         <v>22</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="10" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2009,100 +2008,34 @@
       <c r="A27">
         <v>23</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>144</v>
+      <c r="B27" s="10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>145</v>
+      <c r="B28" s="10" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C40" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="10"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="11"/>
+      <c r="B29" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="6"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2111,11 +2044,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
@@ -2126,232 +2059,232 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2361,59 +2294,59 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B64" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B66" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B68" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2422,7 +2355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H19"/>
   <sheetViews>
@@ -2437,184 +2370,184 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="F2" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="G2" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>134</v>
+        <v>116</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>130</v>
+        <v>118</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="G4" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="H4" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="H5" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>130</v>
+        <v>140</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="F6" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="G6" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="H6" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H7" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2623,12 +2556,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:A21"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2675,7 +2608,7 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -2710,7 +2643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B17"/>
   <sheetViews>
@@ -2722,20 +2655,20 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
@@ -2743,71 +2676,71 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="B8" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B12" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>